<commit_message>
organize old and new VIOLIN input/output formats, clean example folders
</commit_message>
<xml_diff>
--- a/examples/input/Ra4_reading.xlsx
+++ b/examples/input/Ra4_reading.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casey/Framework/VIOLIN/violin_tutorial/test_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaoxiangzhou/Downloads/violin_test/examples/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EB5F9B-4A98-3E40-AF2B-0791711D142E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D895ED70-2E0E-2341-961F-12FD94B98094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="6900" windowWidth="28800" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="118">
   <si>
     <t>inflammation</t>
   </si>
@@ -344,16 +357,53 @@
   </si>
   <si>
     <t>Evidence</t>
+  </si>
+  <si>
+    <t>Database Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Location ID</t>
+  </si>
+  <si>
+    <t>Cell Line</t>
+  </si>
+  <si>
+    <t>Cell Type</t>
+  </si>
+  <si>
+    <t>Organism</t>
+  </si>
+  <si>
+    <t>Positive Reg Location</t>
+  </si>
+  <si>
+    <t>Positive Reg Location ID</t>
+  </si>
+  <si>
+    <t>Negative Reg Location</t>
+  </si>
+  <si>
+    <t>Negative Reg Location ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -379,8 +429,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,56 +734,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>93</v>
       </c>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
       <c r="D1" t="s">
         <v>94</v>
       </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
       <c r="F1" t="s">
-        <v>95</v>
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
       </c>
       <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" t="s">
         <v>101</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>102</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" t="s">
         <v>104</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>105</v>
       </c>
       <c r="V1" t="s">
         <v>106</v>
       </c>
       <c r="W1" t="s">
+        <v>116</v>
+      </c>
+      <c r="X1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y1" t="s">
         <v>97</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>96</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -745,35 +855,35 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="W2" t="s">
-        <v>100</v>
-      </c>
-      <c r="X2" t="s">
-        <v>99</v>
-      </c>
       <c r="Y2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -786,35 +896,35 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>8</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>9</v>
       </c>
-      <c r="W3" t="s">
-        <v>100</v>
-      </c>
-      <c r="X3" t="s">
-        <v>99</v>
-      </c>
       <c r="Y3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -827,35 +937,35 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>7</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>8</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>9</v>
       </c>
-      <c r="W4" t="s">
-        <v>100</v>
-      </c>
-      <c r="X4" t="s">
-        <v>99</v>
-      </c>
       <c r="Y4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -868,35 +978,35 @@
       <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>29</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>7</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>30</v>
       </c>
-      <c r="N5" t="s">
-        <v>15</v>
-      </c>
-      <c r="W5" t="s">
-        <v>100</v>
-      </c>
-      <c r="X5" t="s">
-        <v>99</v>
+      <c r="O5" t="s">
+        <v>15</v>
       </c>
       <c r="Y5" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -909,35 +1019,35 @@
       <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>40</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>41</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>13</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>42</v>
       </c>
-      <c r="N6" t="s">
-        <v>15</v>
-      </c>
-      <c r="W6" t="s">
-        <v>100</v>
-      </c>
-      <c r="X6" t="s">
-        <v>99</v>
+      <c r="O6" t="s">
+        <v>15</v>
       </c>
       <c r="Y6" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -950,35 +1060,35 @@
       <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
         <v>40</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>41</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>13</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>42</v>
       </c>
-      <c r="N7" t="s">
-        <v>15</v>
-      </c>
-      <c r="W7" t="s">
-        <v>100</v>
-      </c>
-      <c r="X7" t="s">
-        <v>99</v>
+      <c r="O7" t="s">
+        <v>15</v>
       </c>
       <c r="Y7" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -991,35 +1101,35 @@
       <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
         <v>46</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>47</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>13</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>48</v>
       </c>
-      <c r="N8" t="s">
-        <v>15</v>
-      </c>
-      <c r="W8" t="s">
-        <v>100</v>
-      </c>
-      <c r="X8" t="s">
-        <v>99</v>
+      <c r="O8" t="s">
+        <v>15</v>
       </c>
       <c r="Y8" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1032,35 +1142,35 @@
       <c r="D9" t="s">
         <v>51</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>52</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>53</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>13</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>54</v>
       </c>
-      <c r="N9" t="s">
-        <v>15</v>
-      </c>
-      <c r="W9" t="s">
-        <v>100</v>
-      </c>
-      <c r="X9" t="s">
-        <v>99</v>
+      <c r="O9" t="s">
+        <v>15</v>
       </c>
       <c r="Y9" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -1073,35 +1183,35 @@
       <c r="D10" t="s">
         <v>85</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>86</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>75</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>60</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>76</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>27</v>
       </c>
-      <c r="W10" t="s">
-        <v>100</v>
-      </c>
-      <c r="X10" t="s">
-        <v>99</v>
-      </c>
       <c r="Y10" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1114,35 +1224,35 @@
       <c r="D11" t="s">
         <v>89</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>63</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>64</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>13</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>65</v>
       </c>
-      <c r="N11" t="s">
-        <v>15</v>
-      </c>
-      <c r="W11" t="s">
-        <v>100</v>
-      </c>
-      <c r="X11" t="s">
-        <v>99</v>
+      <c r="O11" t="s">
+        <v>15</v>
       </c>
       <c r="Y11" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -1155,35 +1265,35 @@
       <c r="D12" t="s">
         <v>85</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>63</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>64</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>13</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>65</v>
       </c>
-      <c r="N12" t="s">
-        <v>15</v>
-      </c>
-      <c r="W12" t="s">
-        <v>100</v>
-      </c>
-      <c r="X12" t="s">
-        <v>99</v>
+      <c r="O12" t="s">
+        <v>15</v>
       </c>
       <c r="Y12" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1196,35 +1306,35 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q13" t="s">
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" t="s">
         <v>19</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>20</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>21</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>22</v>
       </c>
       <c r="V13" t="s">
         <v>9</v>
       </c>
-      <c r="W13" t="s">
-        <v>100</v>
-      </c>
-      <c r="X13" t="s">
-        <v>99</v>
-      </c>
       <c r="Y13" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1237,35 +1347,35 @@
       <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
         <v>27</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>28</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>29</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>7</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>30</v>
       </c>
       <c r="V14" t="s">
         <v>15</v>
       </c>
-      <c r="W14" t="s">
-        <v>100</v>
-      </c>
-      <c r="X14" t="s">
-        <v>99</v>
-      </c>
       <c r="Y14" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1278,35 +1388,35 @@
       <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q15" t="s">
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="R15" t="s">
         <v>28</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>29</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>7</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>30</v>
       </c>
       <c r="V15" t="s">
         <v>15</v>
       </c>
-      <c r="W15" t="s">
-        <v>100</v>
-      </c>
-      <c r="X15" t="s">
-        <v>99</v>
-      </c>
       <c r="Y15" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1319,35 +1429,35 @@
       <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" t="s">
         <v>4</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>58</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>59</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>60</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>61</v>
       </c>
       <c r="V16" t="s">
         <v>15</v>
       </c>
-      <c r="W16" t="s">
-        <v>100</v>
-      </c>
-      <c r="X16" t="s">
-        <v>99</v>
-      </c>
       <c r="Y16" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1360,35 +1470,35 @@
       <c r="D17" t="s">
         <v>65</v>
       </c>
-      <c r="F17" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="R17" t="s">
         <v>66</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>67</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>13</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>68</v>
       </c>
       <c r="V17" t="s">
         <v>15</v>
       </c>
-      <c r="W17" t="s">
-        <v>100</v>
-      </c>
-      <c r="X17" t="s">
-        <v>99</v>
-      </c>
       <c r="Y17" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1401,35 +1511,35 @@
       <c r="D18" t="s">
         <v>71</v>
       </c>
-      <c r="F18" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q18" t="s">
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R18" t="s">
         <v>66</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>67</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>13</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>68</v>
       </c>
       <c r="V18" t="s">
         <v>15</v>
       </c>
-      <c r="W18" t="s">
-        <v>100</v>
-      </c>
-      <c r="X18" t="s">
-        <v>99</v>
-      </c>
       <c r="Y18" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1442,35 +1552,35 @@
       <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="F19" t="s">
+      <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>66</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>67</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>13</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>68</v>
       </c>
       <c r="V19" t="s">
         <v>15</v>
       </c>
-      <c r="W19" t="s">
-        <v>100</v>
-      </c>
-      <c r="X19" t="s">
-        <v>99</v>
-      </c>
       <c r="Y19" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1483,35 +1593,35 @@
       <c r="D20" t="s">
         <v>72</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>74</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>75</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>60</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>76</v>
       </c>
       <c r="V20" t="s">
         <v>27</v>
       </c>
-      <c r="W20" t="s">
-        <v>100</v>
-      </c>
-      <c r="X20" t="s">
-        <v>99</v>
-      </c>
       <c r="Y20" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1524,35 +1634,35 @@
       <c r="D21" t="s">
         <v>80</v>
       </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q21" t="s">
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R21" t="s">
         <v>81</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>82</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>60</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>81</v>
       </c>
       <c r="V21" t="s">
         <v>27</v>
       </c>
-      <c r="W21" t="s">
-        <v>100</v>
-      </c>
-      <c r="X21" t="s">
-        <v>99</v>
-      </c>
       <c r="Y21" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -1565,31 +1675,31 @@
       <c r="D22" t="s">
         <v>92</v>
       </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q22" t="s">
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" t="s">
         <v>72</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>73</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>60</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>72</v>
       </c>
       <c r="V22" t="s">
         <v>27</v>
       </c>
-      <c r="W22" t="s">
-        <v>100</v>
-      </c>
-      <c r="X22" t="s">
-        <v>99</v>
-      </c>
       <c r="Y22" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA22" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>